<commit_message>
fifth commit - base
</commit_message>
<xml_diff>
--- a/data/Registre_des_données.xlsx
+++ b/data/Registre_des_données.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Voirie" sheetId="1" r:id="rId1"/>
@@ -2318,7 +2318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2463,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>